<commit_message>
updated SS_synthetic_data_imbibition_to_Excel.ipynb because the final fit did run into bounds
</commit_message>
<xml_diff>
--- a/python/expdataHISSSimbibition.xlsx
+++ b/python/expdataHISSSimbibition.xlsx
@@ -1561,7 +1561,7 @@
         <v>4.764218811041554</v>
       </c>
       <c r="D2">
-        <v>0.0569314449913351</v>
+        <v>0.05693144499133511</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1575,7 +1575,7 @@
         <v>9.528437622083109</v>
       </c>
       <c r="D3">
-        <v>0.05791418749878328</v>
+        <v>0.05791418749878329</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1603,7 +1603,7 @@
         <v>19.05687524416622</v>
       </c>
       <c r="D5">
-        <v>0.06210800766110168</v>
+        <v>0.06210800766110165</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1631,7 +1631,7 @@
         <v>28.58531286624933</v>
       </c>
       <c r="D7">
-        <v>0.06223782238255264</v>
+        <v>0.06223782238255261</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1645,7 +1645,7 @@
         <v>33.34953167729088</v>
       </c>
       <c r="D8">
-        <v>0.05903592645021518</v>
+        <v>0.05903592645021517</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1673,7 +1673,7 @@
         <v>38.11375048833244</v>
       </c>
       <c r="D10">
-        <v>0.05744835662209536</v>
+        <v>0.0574483566220954</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1701,7 +1701,7 @@
         <v>42.87796929937399</v>
       </c>
       <c r="D12">
-        <v>0.07824745268554013</v>
+        <v>0.07824745268554011</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1715,7 +1715,7 @@
         <v>47.64218811041555</v>
       </c>
       <c r="D13">
-        <v>0.08389125099501911</v>
+        <v>0.08389125099501912</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1729,7 +1729,7 @@
         <v>52.4064069214571</v>
       </c>
       <c r="D14">
-        <v>0.08689159471744119</v>
+        <v>0.08689159471744122</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1757,7 +1757,7 @@
         <v>61.93484454354021</v>
       </c>
       <c r="D16">
-        <v>0.09049271017034721</v>
+        <v>0.09049271017034723</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1771,7 +1771,7 @@
         <v>66.69906335458177</v>
       </c>
       <c r="D17">
-        <v>0.09447176369751389</v>
+        <v>0.09447176369751388</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1785,7 +1785,7 @@
         <v>71.46328216562331</v>
       </c>
       <c r="D18">
-        <v>0.08769483011475017</v>
+        <v>0.0876948301147502</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1799,7 +1799,7 @@
         <v>76.22750097666486</v>
       </c>
       <c r="D19">
-        <v>0.09498976735912848</v>
+        <v>0.09498976735912845</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1813,7 +1813,7 @@
         <v>80.9917197877064</v>
       </c>
       <c r="D20">
-        <v>0.09303673254471519</v>
+        <v>0.09303673254471517</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1827,7 +1827,7 @@
         <v>85.75593859874795</v>
       </c>
       <c r="D21">
-        <v>0.09485985513183144</v>
+        <v>0.09485985513183141</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1841,7 +1841,7 @@
         <v>90.5201574097895</v>
       </c>
       <c r="D22">
-        <v>0.09243775042549808</v>
+        <v>0.09243775042549807</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1855,7 +1855,7 @@
         <v>95.28437622083105</v>
       </c>
       <c r="D23">
-        <v>0.09410658219629567</v>
+        <v>0.09410658219629565</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1869,7 +1869,7 @@
         <v>100.0485950318726</v>
       </c>
       <c r="D24">
-        <v>0.09021738047535705</v>
+        <v>0.09021738047535706</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1883,7 +1883,7 @@
         <v>104.8128138429142</v>
       </c>
       <c r="D25">
-        <v>0.09033185294969005</v>
+        <v>0.09033185294969007</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1911,7 +1911,7 @@
         <v>114.3412514649972</v>
       </c>
       <c r="D27">
-        <v>0.09363998334154294</v>
+        <v>0.09363998334154293</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1939,7 +1939,7 @@
         <v>123.8696890870803</v>
       </c>
       <c r="D29">
-        <v>0.08945552293645186</v>
+        <v>0.08945552293645187</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1953,7 +1953,7 @@
         <v>128.6339078981219</v>
       </c>
       <c r="D30">
-        <v>0.09513286577622426</v>
+        <v>0.09513286577622423</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1967,7 +1967,7 @@
         <v>133.3981267091635</v>
       </c>
       <c r="D31">
-        <v>0.09489075655453465</v>
+        <v>0.09489075655453462</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1981,7 +1981,7 @@
         <v>138.162345520205</v>
       </c>
       <c r="D32">
-        <v>0.09032557588388958</v>
+        <v>0.09032557588388959</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1995,7 +1995,7 @@
         <v>142.9265643312466</v>
       </c>
       <c r="D33">
-        <v>0.0926590568557199</v>
+        <v>0.09265905685571989</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2009,7 +2009,7 @@
         <v>147.6907831422881</v>
       </c>
       <c r="D34">
-        <v>0.0897136746508225</v>
+        <v>0.08971367465082251</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2023,7 +2023,7 @@
         <v>152.4550019533297</v>
       </c>
       <c r="D35">
-        <v>0.0891607798763344</v>
+        <v>0.08916077987633442</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2037,7 +2037,7 @@
         <v>153.1339031339031</v>
       </c>
       <c r="D36">
-        <v>0.09022387586840232</v>
+        <v>0.09022387586840233</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2065,7 +2065,7 @@
         <v>161.9834395754128</v>
       </c>
       <c r="D38">
-        <v>0.1284347727725782</v>
+        <v>0.1284347727725781</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2121,7 +2121,7 @@
         <v>181.040314819579</v>
       </c>
       <c r="D42">
-        <v>0.1252027580148524</v>
+        <v>0.1252027580148525</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2191,7 +2191,7 @@
         <v>204.8614088747867</v>
       </c>
       <c r="D47">
-        <v>0.1225058708746559</v>
+        <v>0.122505870874656</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2331,7 +2331,7 @@
         <v>252.5035969852022</v>
       </c>
       <c r="D57">
-        <v>0.1244867636821466</v>
+        <v>0.1244867636821467</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2597,7 +2597,7 @@
         <v>333.495316772909</v>
       </c>
       <c r="D76">
-        <v>0.1882611917817125</v>
+        <v>0.1882611917817127</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2737,7 +2737,7 @@
         <v>381.1375048833247</v>
       </c>
       <c r="D86">
-        <v>0.1885899848366532</v>
+        <v>0.1885899848366533</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2779,7 +2779,7 @@
         <v>395.4301613164494</v>
       </c>
       <c r="D89">
-        <v>0.1937746670871025</v>
+        <v>0.1937746670871024</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2961,7 +2961,7 @@
         <v>452.6007870489483</v>
       </c>
       <c r="D102">
-        <v>0.2203172686671135</v>
+        <v>0.2203172686671134</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2989,7 +2989,7 @@
         <v>462.1292246710315</v>
       </c>
       <c r="D104">
-        <v>0.2156123309742109</v>
+        <v>0.215612330974211</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3297,7 +3297,7 @@
         <v>562.1778197029046</v>
       </c>
       <c r="D126">
-        <v>0.2418378616873208</v>
+        <v>0.2418378616873207</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3311,7 +3311,7 @@
         <v>566.9420385139462</v>
       </c>
       <c r="D127">
-        <v>0.2412859149117888</v>
+        <v>0.2412859149117887</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3395,7 +3395,7 @@
         <v>595.5273513801956</v>
       </c>
       <c r="D133">
-        <v>0.2345340295176499</v>
+        <v>0.23453402951765</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3549,7 +3549,7 @@
         <v>647.9337583016529</v>
       </c>
       <c r="D144">
-        <v>0.2407915301285381</v>
+        <v>0.240791530128538</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -3675,7 +3675,7 @@
         <v>686.0475087899854</v>
       </c>
       <c r="D153">
-        <v>0.2134674024764478</v>
+        <v>0.2134674024764477</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3955,7 +3955,7 @@
         <v>781.331885010817</v>
       </c>
       <c r="D173">
-        <v>0.2077301291632979</v>
+        <v>0.207730129163298</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -3983,7 +3983,7 @@
         <v>787.7492877492899</v>
       </c>
       <c r="D175">
-        <v>0.2137903973277685</v>
+        <v>0.2137903973277684</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -4011,7 +4011,7 @@
         <v>795.6245414439417</v>
       </c>
       <c r="D177">
-        <v>0.1908363364538694</v>
+        <v>0.1908363364538695</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -4039,7 +4039,7 @@
         <v>805.1529790660248</v>
       </c>
       <c r="D179">
-        <v>0.1907106283328062</v>
+        <v>0.1907106283328063</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -4123,7 +4123,7 @@
         <v>833.7382919322744</v>
       </c>
       <c r="D185">
-        <v>0.1962054483871754</v>
+        <v>0.1962054483871753</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4193,7 +4193,7 @@
         <v>857.5593859874822</v>
       </c>
       <c r="D190">
-        <v>0.1971874262466216</v>
+        <v>0.1971874262466215</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -4207,7 +4207,7 @@
         <v>862.3236047985238</v>
       </c>
       <c r="D191">
-        <v>0.1943321630747997</v>
+        <v>0.1943321630747996</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -4277,7 +4277,7 @@
         <v>886.1446988537317</v>
       </c>
       <c r="D196">
-        <v>0.1898188866371805</v>
+        <v>0.1898188866371806</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -4319,7 +4319,7 @@
         <v>900.4373552868564</v>
       </c>
       <c r="D199">
-        <v>0.1956596019555063</v>
+        <v>0.1956596019555062</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -4431,7 +4431,7 @@
         <v>933.7868869641475</v>
       </c>
       <c r="D207">
-        <v>0.170479976236255</v>
+        <v>0.1704799762362549</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -4445,7 +4445,7 @@
         <v>938.5511057751891</v>
       </c>
       <c r="D208">
-        <v>0.1666228583526526</v>
+        <v>0.1666228583526527</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -4473,7 +4473,7 @@
         <v>948.0795433972722</v>
       </c>
       <c r="D210">
-        <v>0.1711801106882233</v>
+        <v>0.1711801106882235</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -4487,7 +4487,7 @@
         <v>952.8437622083138</v>
       </c>
       <c r="D211">
-        <v>0.166183361535115</v>
+        <v>0.1661833615351151</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -4543,7 +4543,7 @@
         <v>971.9006374524799</v>
       </c>
       <c r="D215">
-        <v>0.172216959794379</v>
+        <v>0.1722169597943789</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -4613,7 +4613,7 @@
         <v>995.7217315076879</v>
       </c>
       <c r="D220">
-        <v>0.1726851064108451</v>
+        <v>0.172685106410845</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -4669,7 +4669,7 @@
         <v>1014.778606751854</v>
       </c>
       <c r="D224">
-        <v>0.1677140378027256</v>
+        <v>0.1677140378027257</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -4683,7 +4683,7 @@
         <v>1019.542825562896</v>
       </c>
       <c r="D225">
-        <v>0.1732671635258974</v>
+        <v>0.1732671635258973</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -4767,7 +4767,7 @@
         <v>1043.363919618103</v>
       </c>
       <c r="D231">
-        <v>0.1556832781149677</v>
+        <v>0.1556832781149678</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -4781,7 +4781,7 @@
         <v>1048.128138429145</v>
       </c>
       <c r="D232">
-        <v>0.1571322053052839</v>
+        <v>0.157132205305284</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -4949,7 +4949,7 @@
         <v>1105.298764161643</v>
       </c>
       <c r="D244">
-        <v>0.1631610495298675</v>
+        <v>0.1631610495298674</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -5173,7 +5173,7 @@
         <v>1181.526265138306</v>
       </c>
       <c r="D260">
-        <v>0.1552988281222717</v>
+        <v>0.1552988281222718</v>
       </c>
     </row>
     <row r="261" spans="1:4">
@@ -5215,7 +5215,7 @@
         <v>1196.924220335592</v>
       </c>
       <c r="D263">
-        <v>0.2529324005374691</v>
+        <v>0.2529324005374692</v>
       </c>
     </row>
     <row r="264" spans="1:4">
@@ -5285,7 +5285,7 @@
         <v>1244.566408446008</v>
       </c>
       <c r="D268">
-        <v>0.2479756457900794</v>
+        <v>0.2479756457900795</v>
       </c>
     </row>
     <row r="269" spans="1:4">
@@ -5299,7 +5299,7 @@
         <v>1254.094846068091</v>
       </c>
       <c r="D269">
-        <v>0.2489685620084341</v>
+        <v>0.2489685620084342</v>
       </c>
     </row>
     <row r="270" spans="1:4">
@@ -5341,7 +5341,7 @@
         <v>1282.680158934341</v>
       </c>
       <c r="D272">
-        <v>0.2493336275581154</v>
+        <v>0.2493336275581156</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -5453,7 +5453,7 @@
         <v>1358.907659911006</v>
       </c>
       <c r="D280">
-        <v>0.2521941840796207</v>
+        <v>0.2521941840796205</v>
       </c>
     </row>
     <row r="281" spans="1:4">
@@ -5467,7 +5467,7 @@
         <v>1363.247863247865</v>
       </c>
       <c r="D281">
-        <v>0.247248251416065</v>
+        <v>0.2472482514160648</v>
       </c>
     </row>
     <row r="282" spans="1:4">
@@ -5481,7 +5481,7 @@
         <v>1376.218448960925</v>
       </c>
       <c r="D282">
-        <v>0.5333460207524745</v>
+        <v>0.5333460207524712</v>
       </c>
     </row>
     <row r="283" spans="1:4">
@@ -5495,7 +5495,7 @@
         <v>1400.039543016133</v>
       </c>
       <c r="D283">
-        <v>0.5111859077375281</v>
+        <v>0.511185907737528</v>
       </c>
     </row>
     <row r="284" spans="1:4">
@@ -5509,7 +5509,7 @@
         <v>1423.860637071341</v>
       </c>
       <c r="D284">
-        <v>0.5063492935144125</v>
+        <v>0.506349293514412</v>
       </c>
     </row>
     <row r="285" spans="1:4">
@@ -5523,7 +5523,7 @@
         <v>1447.681731126548</v>
       </c>
       <c r="D285">
-        <v>0.5087591315338031</v>
+        <v>0.5087591315338049</v>
       </c>
     </row>
     <row r="286" spans="1:4">
@@ -5537,7 +5537,7 @@
         <v>1471.502825181756</v>
       </c>
       <c r="D286">
-        <v>0.5011310751463351</v>
+        <v>0.5011310751463356</v>
       </c>
     </row>
     <row r="287" spans="1:4">
@@ -5551,7 +5551,7 @@
         <v>1495.323919236964</v>
       </c>
       <c r="D287">
-        <v>0.5055410884809219</v>
+        <v>0.5055410884809188</v>
       </c>
     </row>
     <row r="288" spans="1:4">
@@ -5565,7 +5565,7 @@
         <v>1519.145013292172</v>
       </c>
       <c r="D288">
-        <v>0.5070075218920053</v>
+        <v>0.5070075218920039</v>
       </c>
     </row>
     <row r="289" spans="1:4">
@@ -5579,7 +5579,7 @@
         <v>1542.96610734738</v>
       </c>
       <c r="D289">
-        <v>0.5057602785227077</v>
+        <v>0.5057602785227132</v>
       </c>
     </row>
     <row r="290" spans="1:4">
@@ -5593,7 +5593,7 @@
         <v>1566.787201402587</v>
       </c>
       <c r="D290">
-        <v>0.5041456402754814</v>
+        <v>0.5041456402754863</v>
       </c>
     </row>
     <row r="291" spans="1:4">
@@ -5607,7 +5607,7 @@
         <v>1590.608295457795</v>
       </c>
       <c r="D291">
-        <v>0.5059689510785631</v>
+        <v>0.5059689510785653</v>
       </c>
     </row>
     <row r="292" spans="1:4">
@@ -5621,7 +5621,7 @@
         <v>1614.429389513003</v>
       </c>
       <c r="D292">
-        <v>0.5015106420638963</v>
+        <v>0.5015106420638981</v>
       </c>
     </row>
     <row r="293" spans="1:4">
@@ -5635,7 +5635,7 @@
         <v>1638.250483568211</v>
       </c>
       <c r="D293">
-        <v>0.5050276967445867</v>
+        <v>0.5050276967445875</v>
       </c>
     </row>
     <row r="294" spans="1:4">
@@ -5649,7 +5649,7 @@
         <v>1662.071577623419</v>
       </c>
       <c r="D294">
-        <v>0.5007371617486347</v>
+        <v>0.5007371617486343</v>
       </c>
     </row>
     <row r="295" spans="1:4">
@@ -5663,7 +5663,7 @@
         <v>1685.892671678627</v>
       </c>
       <c r="D295">
-        <v>0.5053713730304572</v>
+        <v>0.5053713730304573</v>
       </c>
     </row>
     <row r="296" spans="1:4">
@@ -5677,7 +5677,7 @@
         <v>1709.713765733834</v>
       </c>
       <c r="D296">
-        <v>0.4989600966851285</v>
+        <v>0.4989600966851288</v>
       </c>
     </row>
     <row r="297" spans="1:4">
@@ -5691,7 +5691,7 @@
         <v>1733.534859789042</v>
       </c>
       <c r="D297">
-        <v>0.5053941183492204</v>
+        <v>0.50539411834922</v>
       </c>
     </row>
     <row r="298" spans="1:4">
@@ -5705,7 +5705,7 @@
         <v>1757.35595384425</v>
       </c>
       <c r="D298">
-        <v>0.5044999140060678</v>
+        <v>0.5044999140060673</v>
       </c>
     </row>
     <row r="299" spans="1:4">
@@ -5719,7 +5719,7 @@
         <v>1781.177047899458</v>
       </c>
       <c r="D299">
-        <v>0.5045958303720256</v>
+        <v>0.5045958303720252</v>
       </c>
     </row>
     <row r="300" spans="1:4">
@@ -5733,7 +5733,7 @@
         <v>1804.998141954666</v>
       </c>
       <c r="D300">
-        <v>0.4986913737977337</v>
+        <v>0.4986913737977341</v>
       </c>
     </row>
     <row r="301" spans="1:4">
@@ -5747,7 +5747,7 @@
         <v>1828.819236009874</v>
       </c>
       <c r="D301">
-        <v>0.5025425366654157</v>
+        <v>0.5025425366654177</v>
       </c>
     </row>
     <row r="302" spans="1:4">
@@ -5761,7 +5761,7 @@
         <v>1852.64033006508</v>
       </c>
       <c r="D302">
-        <v>0.4978021360533416</v>
+        <v>0.4978021360533487</v>
       </c>
     </row>
     <row r="303" spans="1:4">
@@ -5775,7 +5775,7 @@
         <v>1876.461424120288</v>
       </c>
       <c r="D303">
-        <v>0.5035523443784675</v>
+        <v>0.5035523443784661</v>
       </c>
     </row>
     <row r="304" spans="1:4">
@@ -5789,7 +5789,7 @@
         <v>1900.282518175496</v>
       </c>
       <c r="D304">
-        <v>0.4977256281329018</v>
+        <v>0.4977256281328986</v>
       </c>
     </row>
     <row r="305" spans="1:4">
@@ -5803,7 +5803,7 @@
         <v>1924.103612230704</v>
       </c>
       <c r="D305">
-        <v>0.4983531642157283</v>
+        <v>0.4983531642157247</v>
       </c>
     </row>
     <row r="306" spans="1:4">
@@ -5817,7 +5817,7 @@
         <v>1947.924706285912</v>
       </c>
       <c r="D306">
-        <v>0.4995003288440562</v>
+        <v>0.4995003288440526</v>
       </c>
     </row>
     <row r="307" spans="1:4">
@@ -5831,7 +5831,7 @@
         <v>1971.74580034112</v>
       </c>
       <c r="D307">
-        <v>0.5048026976772061</v>
+        <v>0.5048026976772041</v>
       </c>
     </row>
     <row r="308" spans="1:4">
@@ -5845,7 +5845,7 @@
         <v>1995.566894396327</v>
       </c>
       <c r="D308">
-        <v>0.5006259933466554</v>
+        <v>0.5006259933466547</v>
       </c>
     </row>
     <row r="309" spans="1:4">
@@ -5859,7 +5859,7 @@
         <v>2019.387988451535</v>
       </c>
       <c r="D309">
-        <v>0.5020654511651347</v>
+        <v>0.5020654511651333</v>
       </c>
     </row>
     <row r="310" spans="1:4">
@@ -5873,7 +5873,7 @@
         <v>2043.209082506743</v>
       </c>
       <c r="D310">
-        <v>0.5022948694745438</v>
+        <v>0.5022948694745394</v>
       </c>
     </row>
     <row r="311" spans="1:4">
@@ -5887,7 +5887,7 @@
         <v>2067.030176561951</v>
       </c>
       <c r="D311">
-        <v>0.4994974675747374</v>
+        <v>0.4994974675747356</v>
       </c>
     </row>
     <row r="312" spans="1:4">
@@ -5901,7 +5901,7 @@
         <v>2090.851270617158</v>
       </c>
       <c r="D312">
-        <v>0.5023274715301944</v>
+        <v>0.5023274715301935</v>
       </c>
     </row>
     <row r="313" spans="1:4">
@@ -5915,7 +5915,7 @@
         <v>2114.672364672366</v>
       </c>
       <c r="D313">
-        <v>0.5030523155075464</v>
+        <v>0.5030523155075459</v>
       </c>
     </row>
   </sheetData>
@@ -6153,7 +6153,7 @@
         <v>0.8199151069799721</v>
       </c>
       <c r="P2">
-        <v>0.8365044627746999</v>
+        <v>0.8365044627747059</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -6200,10 +6200,10 @@
         <v>0.7834489463721713</v>
       </c>
       <c r="O3">
-        <v>0.811480292845713</v>
+        <v>0.8114802928457131</v>
       </c>
       <c r="P3">
-        <v>0.8457341730656646</v>
+        <v>0.84573417306567</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -6253,7 +6253,7 @@
         <v>0.8103263470548944</v>
       </c>
       <c r="P4">
-        <v>0.840563682640926</v>
+        <v>0.8405636826409313</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -6300,10 +6300,10 @@
         <v>0.7697410673402796</v>
       </c>
       <c r="O5">
-        <v>0.8037872479974311</v>
+        <v>0.8037872479974312</v>
       </c>
       <c r="P5">
-        <v>0.8460915344704385</v>
+        <v>0.8460915344704428</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -6353,7 +6353,7 @@
         <v>0.8174043008266227</v>
       </c>
       <c r="P6">
-        <v>0.8297675859049982</v>
+        <v>0.829767585905003</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -6400,10 +6400,10 @@
         <v>0.7657149162486658</v>
       </c>
       <c r="O7">
-        <v>0.8221752714290061</v>
+        <v>0.822175271429006</v>
       </c>
       <c r="P7">
-        <v>0.8339163216082297</v>
+        <v>0.8339163216082338</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -6453,7 +6453,7 @@
         <v>0.807695591546069</v>
       </c>
       <c r="P8">
-        <v>0.8445333703462481</v>
+        <v>0.8445333703462514</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -6500,10 +6500,10 @@
         <v>0.7678277934546237</v>
       </c>
       <c r="O9">
-        <v>0.8014906178612495</v>
+        <v>0.8014906178612498</v>
       </c>
       <c r="P9">
-        <v>0.8440047090668548</v>
+        <v>0.8440047090668573</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -6550,10 +6550,10 @@
         <v>0.7739356854419296</v>
       </c>
       <c r="O10">
-        <v>0.7995776591291011</v>
+        <v>0.7995776591291012</v>
       </c>
       <c r="P10">
-        <v>0.8361486656366643</v>
+        <v>0.8361486656366673</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -6600,10 +6600,10 @@
         <v>0.7800357337041901</v>
       </c>
       <c r="O11">
-        <v>0.8109631204426314</v>
+        <v>0.810963120442631</v>
       </c>
       <c r="P11">
-        <v>0.8401483628757095</v>
+        <v>0.8401483628757114</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -6650,10 +6650,10 @@
         <v>0.7804446591542684</v>
       </c>
       <c r="O12">
-        <v>0.8178437911583073</v>
+        <v>0.8178437911583069</v>
       </c>
       <c r="P12">
-        <v>0.8482543834139918</v>
+        <v>0.8482543834139941</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -6700,10 +6700,10 @@
         <v>0.7595799992780788</v>
       </c>
       <c r="O13">
-        <v>0.8107776885027853</v>
+        <v>0.8107776885027849</v>
       </c>
       <c r="P13">
-        <v>0.8389391090888112</v>
+        <v>0.8389391090888132</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -6750,10 +6750,10 @@
         <v>0.7665716198255355</v>
       </c>
       <c r="O14">
-        <v>0.7923778130660497</v>
+        <v>0.7923778130660494</v>
       </c>
       <c r="P14">
-        <v>0.8252941262563877</v>
+        <v>0.8252941262563893</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -6800,10 +6800,10 @@
         <v>0.7669864229156174</v>
       </c>
       <c r="O15">
-        <v>0.8124927118423505</v>
+        <v>0.8124927118423502</v>
       </c>
       <c r="P15">
-        <v>0.8362504816122132</v>
+        <v>0.8362504816122144</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -6850,10 +6850,10 @@
         <v>0.7625358663940239</v>
       </c>
       <c r="O16">
-        <v>0.7926538366961762</v>
+        <v>0.7926538366961758</v>
       </c>
       <c r="P16">
-        <v>0.8220043079380509</v>
+        <v>0.8220043079380527</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -6900,10 +6900,10 @@
         <v>0.7555977131664136</v>
       </c>
       <c r="O17">
-        <v>0.8042058815346546</v>
+        <v>0.8042058815346542</v>
       </c>
       <c r="P17">
-        <v>0.8293937817671699</v>
+        <v>0.829393781767171</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -6950,10 +6950,10 @@
         <v>0.7548817439478162</v>
       </c>
       <c r="O18">
-        <v>0.7976365590423046</v>
+        <v>0.7976365590423041</v>
       </c>
       <c r="P18">
-        <v>0.8254793306452265</v>
+        <v>0.8254793306452278</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -7000,10 +7000,10 @@
         <v>0.7514942739488643</v>
       </c>
       <c r="O19">
-        <v>0.7996979594014092</v>
+        <v>0.7996979594014088</v>
       </c>
       <c r="P19">
-        <v>0.8431266987604231</v>
+        <v>0.843126698760425</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -7050,10 +7050,10 @@
         <v>0.7579420507788072</v>
       </c>
       <c r="O20">
-        <v>0.785211303550444</v>
+        <v>0.7852113035504436</v>
       </c>
       <c r="P20">
-        <v>0.8178519465387259</v>
+        <v>0.8178519465387267</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -7100,10 +7100,10 @@
         <v>0.7429014050765371</v>
       </c>
       <c r="O21">
-        <v>0.7951530335510373</v>
+        <v>0.7951530335510369</v>
       </c>
       <c r="P21">
-        <v>0.8297009008340367</v>
+        <v>0.8297009008340376</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -7150,10 +7150,10 @@
         <v>0.7407513790973054</v>
       </c>
       <c r="O22">
-        <v>0.7798157911766764</v>
+        <v>0.7798157911766761</v>
       </c>
       <c r="P22">
-        <v>0.8366162283297427</v>
+        <v>0.8366162283297431</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -7200,10 +7200,10 @@
         <v>0.747500373132755</v>
       </c>
       <c r="O23">
-        <v>0.7759748292317633</v>
+        <v>0.7759748292317634</v>
       </c>
       <c r="P23">
-        <v>0.8233715941613384</v>
+        <v>0.8233715941613385</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -7250,10 +7250,10 @@
         <v>0.7548920804720659</v>
       </c>
       <c r="O24">
-        <v>0.7921643985793932</v>
+        <v>0.7921643985793934</v>
       </c>
       <c r="P24">
-        <v>0.8357996060161609</v>
+        <v>0.835799606016161</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -7303,7 +7303,7 @@
         <v>0.7845520345537872</v>
       </c>
       <c r="P25">
-        <v>0.8354991512551604</v>
+        <v>0.8354991512551605</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -7350,10 +7350,10 @@
         <v>0.7439782543434234</v>
       </c>
       <c r="O26">
-        <v>0.7747583392861785</v>
+        <v>0.7747583392861787</v>
       </c>
       <c r="P26">
-        <v>0.8326645486365934</v>
+        <v>0.8326645486365931</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -7400,10 +7400,10 @@
         <v>0.7311771055507938</v>
       </c>
       <c r="O27">
-        <v>0.7873355901290234</v>
+        <v>0.7873355901290235</v>
       </c>
       <c r="P27">
-        <v>0.8322147713128675</v>
+        <v>0.8322147713128677</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -7450,10 +7450,10 @@
         <v>0.7193464483951391</v>
       </c>
       <c r="O28">
-        <v>0.762659798206258</v>
+        <v>0.7626597982062582</v>
       </c>
       <c r="P28">
-        <v>0.8170274178337412</v>
+        <v>0.8170274178337417</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -7500,10 +7500,10 @@
         <v>0.7295340294366393</v>
       </c>
       <c r="O29">
-        <v>0.772186917207121</v>
+        <v>0.7721869172071212</v>
       </c>
       <c r="P29">
-        <v>0.8118725037316533</v>
+        <v>0.8118725037316534</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -7550,10 +7550,10 @@
         <v>0.7300176464331187</v>
       </c>
       <c r="O30">
-        <v>0.7599701544129794</v>
+        <v>0.7599701544129797</v>
       </c>
       <c r="P30">
-        <v>0.8046233917416938</v>
+        <v>0.8046233917416941</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -7600,7 +7600,7 @@
         <v>0.7297816719254216</v>
       </c>
       <c r="O31">
-        <v>0.7736949177963353</v>
+        <v>0.7736949177963354</v>
       </c>
       <c r="P31">
         <v>0.8207054096402427</v>
@@ -7650,10 +7650,10 @@
         <v>0.7203893298839062</v>
       </c>
       <c r="O32">
-        <v>0.7648471212344435</v>
+        <v>0.7648471212344438</v>
       </c>
       <c r="P32">
-        <v>0.8048001854676706</v>
+        <v>0.804800185467671</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -7700,10 +7700,10 @@
         <v>0.6994805170134446</v>
       </c>
       <c r="O33">
-        <v>0.7547474753407111</v>
+        <v>0.7547474753407113</v>
       </c>
       <c r="P33">
-        <v>0.8155806361243089</v>
+        <v>0.8155806361243086</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -7753,7 +7753,7 @@
         <v>0.7456462917492618</v>
       </c>
       <c r="P34">
-        <v>0.7965423445486561</v>
+        <v>0.796542344548656</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -7800,10 +7800,10 @@
         <v>0.6987528930718692</v>
       </c>
       <c r="O35">
-        <v>0.7364198060862949</v>
+        <v>0.736419806086295</v>
       </c>
       <c r="P35">
-        <v>0.7894954356815121</v>
+        <v>0.7894954356815119</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -7853,7 +7853,7 @@
         <v>0.7483923415234789</v>
       </c>
       <c r="P36">
-        <v>0.8054690453324822</v>
+        <v>0.8054690453324819</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -7900,10 +7900,10 @@
         <v>0.6862468697620581</v>
       </c>
       <c r="O37">
-        <v>0.738499551632973</v>
+        <v>0.7384995516329731</v>
       </c>
       <c r="P37">
-        <v>0.7849491435446508</v>
+        <v>0.7849491435446504</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -8003,7 +8003,7 @@
         <v>0.7257959310419457</v>
       </c>
       <c r="P39">
-        <v>0.7936895532383506</v>
+        <v>0.7936895532383507</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -8050,10 +8050,10 @@
         <v>0.6595921304629904</v>
       </c>
       <c r="O40">
-        <v>0.715664399370756</v>
+        <v>0.7156643993707559</v>
       </c>
       <c r="P40">
-        <v>0.769097543829812</v>
+        <v>0.7690975438298121</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -8103,7 +8103,7 @@
         <v>0.7182447032999768</v>
       </c>
       <c r="P41">
-        <v>0.7798083445456846</v>
+        <v>0.7798083445456845</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -8203,7 +8203,7 @@
         <v>0.6895537249539323</v>
       </c>
       <c r="P43">
-        <v>0.7394652950698754</v>
+        <v>0.7394652950698751</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -8253,7 +8253,7 @@
         <v>0.6583980206228548</v>
       </c>
       <c r="P44">
-        <v>0.729719923172937</v>
+        <v>0.7297199231729371</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -8276,7 +8276,7 @@
         <v>0.2611718542010664</v>
       </c>
       <c r="G45">
-        <v>0.320700323421281</v>
+        <v>0.3207003234212809</v>
       </c>
       <c r="H45">
         <v>0.3766263379594102</v>
@@ -8303,7 +8303,7 @@
         <v>0.6541820191040258</v>
       </c>
       <c r="P45">
-        <v>0.7267885076620313</v>
+        <v>0.7267885076620315</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -8353,7 +8353,7 @@
         <v>0.6214290200324888</v>
       </c>
       <c r="P46">
-        <v>0.6994631659126231</v>
+        <v>0.6994631659126233</v>
       </c>
     </row>
     <row r="47" spans="1:16">

</xml_diff>